<commit_message>
Updated the Investment-Spreadsheet and the fond_id's for Optimization
</commit_message>
<xml_diff>
--- a/Investment_Produkte_Details.xlsx
+++ b/Investment_Produkte_Details.xlsx
@@ -9,30 +9,31 @@
   </bookViews>
   <sheets>
     <sheet name="Allgemeines" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Kapital Plus A EUR" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Jupiter Europa L EUR B" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Mozart one R T" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Fidelity Fd.Glob.Technology" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="iShares ETF" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Fidelity Funds Germany" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="M&amp;G European Strategic Value C " sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Deutsche Invest I German Eq.FC " sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="BGF European Special Situati." sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="BGF Cont.European" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Fidelity Funds" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="BSF European Opport.Extension " sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="MainFirst Germany C" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="MSIF US Growth Z EUR" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="BGF World Technology" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Sheet2" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="MSIF Asia Opportunity AH EUR" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Sheet19" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Kapital Plus A EUR" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Jupiter Europa L EUR B" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Mozart one R T" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Fidelity Fd.Glob.Technology" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="iShares ETF" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Fidelity Funds Germany" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="M&amp;G European Strategic Value C " sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Deutsche Invest I German Eq.FC " sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="BGF European Special Situati." sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="BGF Cont.European" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Fidelity Funds" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="BSF European Opport.Extension " sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="MainFirst Germany C" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="MSIF US Growth Z EUR" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="BGF World Technology" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Sheet2" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="MSIF Asia Opportunity AH EUR" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="198">
   <si>
     <t>Fond Name</t>
   </si>
@@ -49,6 +50,12 @@
     <t>Morningstar Fond_ID</t>
   </si>
   <si>
+    <t>Kaufbar (Hellobank)</t>
+  </si>
+  <si>
+    <t>Mindest?</t>
+  </si>
+  <si>
     <t>3 Banken Österreich-Fonds</t>
   </si>
   <si>
@@ -82,6 +89,9 @@
     <t>F00000X0M9</t>
   </si>
   <si>
+    <t>Ja, Morgan Stanley</t>
+  </si>
+  <si>
     <t>BGF World Technology</t>
   </si>
   <si>
@@ -100,6 +110,9 @@
     <t>0P0000VHOL</t>
   </si>
   <si>
+    <t>Ja, Blackrock</t>
+  </si>
+  <si>
     <t>MSIF US Growth Z EUR</t>
   </si>
   <si>
@@ -136,6 +149,9 @@
     <t>F000002J6W</t>
   </si>
   <si>
+    <t>Ja, Fondsgesellschaft</t>
+  </si>
+  <si>
     <t>BSF European Opport.Extension </t>
   </si>
   <si>
@@ -151,6 +167,9 @@
     <t>F0000045M3</t>
   </si>
   <si>
+    <t>Nein, Institutioneller</t>
+  </si>
+  <si>
     <t>Fidelity Funds - Global Technology Fund</t>
   </si>
   <si>
@@ -196,6 +215,12 @@
     <t>F0000020MG</t>
   </si>
   <si>
+    <t>Berechnungskurs komisch!</t>
+  </si>
+  <si>
+    <t>1500???</t>
+  </si>
+  <si>
     <t>Odey European Focus Fund B</t>
   </si>
   <si>
@@ -220,12 +245,15 @@
     <t>https://kurse.hellobank.at/k/fonds/fondsdetail.aspx?id=FU_100033448</t>
   </si>
   <si>
-    <t>Aktien Europa (ohne GBT) Standardwerte </t>
+    <t>Aktien Europa (ohne GBT) Standardwerte</t>
   </si>
   <si>
     <t>F00000MGKD</t>
   </si>
   <si>
+    <t>Nein, nicht gefunden</t>
+  </si>
+  <si>
     <t>BGF European Special Situati.</t>
   </si>
   <si>
@@ -304,6 +332,12 @@
     <t>0P0000M7TK</t>
   </si>
   <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
     <t>Fidelity Fd.Glob.Technology A Dis EUR </t>
   </si>
   <si>
@@ -322,6 +356,9 @@
     <t>F0GBR04D20</t>
   </si>
   <si>
+    <t>Ja, Fidelity</t>
+  </si>
+  <si>
     <t>Mozart one R T</t>
   </si>
   <si>
@@ -337,6 +374,9 @@
     <t>F00000JRBY</t>
   </si>
   <si>
+    <t>Zu Ö-Lastig</t>
+  </si>
+  <si>
     <t>MEAG EuroBalance</t>
   </si>
   <si>
@@ -382,7 +422,10 @@
     <t>F0GBR04CIW</t>
   </si>
   <si>
-    <t>Vanguard U.S. 500 Stock Index Fund Investor </t>
+    <t>Ja, Baaderbank</t>
+  </si>
+  <si>
+    <t>Vanguard U.S. 500 Stock Index Fund Investor</t>
   </si>
   <si>
     <t>IE0032620787</t>
@@ -394,7 +437,7 @@
     <t>F0GBR04G0F</t>
   </si>
   <si>
-    <t>Frankfurter Aktienfonds f.Stiftungen T </t>
+    <t>Frankfurter Aktienfonds f.Stiftungen T</t>
   </si>
   <si>
     <t>DE000A0M8HD2</t>
@@ -409,7 +452,7 @@
     <t>F0000020H2</t>
   </si>
   <si>
-    <t>JPMorgan Funds - US Small Cap Growth Fund A </t>
+    <t>JPMorgan Funds - US Small Cap Growth Fund A</t>
   </si>
   <si>
     <t>LU0401357743</t>
@@ -439,58 +482,130 @@
     <t>FOND ID</t>
   </si>
   <si>
+    <t>Name Detail</t>
+  </si>
+  <si>
     <t>F000000IK5</t>
   </si>
   <si>
     <t>LU0313923228</t>
   </si>
   <si>
+    <t>BlackRock Str.Fds-Eur.Opp.Ext.</t>
+  </si>
+  <si>
+    <t>Ja, Börse</t>
+  </si>
+  <si>
     <t>F0GBR06DWD</t>
   </si>
   <si>
     <t>LU0148742835</t>
   </si>
   <si>
+    <t>Deutsche Multi Opportunities</t>
+  </si>
+  <si>
+    <t>Ja, Direkthandel Baaderbank</t>
+  </si>
+  <si>
     <t>F00000T4KE</t>
   </si>
   <si>
     <t>LU1038809395</t>
   </si>
   <si>
+    <t>FLOSSBACH V STORCH</t>
+  </si>
+  <si>
+    <t>Ja, FLOSSBACH V STORCH</t>
+  </si>
+  <si>
     <t>F00000V70D</t>
   </si>
   <si>
     <t>DE000A12BPP4</t>
   </si>
   <si>
+    <t>Frankfurter Aktienfonds für Stiftungen TI</t>
+  </si>
+  <si>
+    <t>Ja, PEH</t>
+  </si>
+  <si>
     <t>F0000007LD</t>
   </si>
   <si>
     <t>GB00B1VMCY93</t>
   </si>
   <si>
+    <t>M&amp;G OPTIMAL INCOME FUND (T)</t>
+  </si>
+  <si>
+    <t>Ja, M &amp; G INVESTMENTS</t>
+  </si>
+  <si>
     <t>F00000LNTR</t>
   </si>
   <si>
     <t>LU0552385618</t>
   </si>
   <si>
+    <t>Morgan Stanley Global Opp A Hedged EUR</t>
+  </si>
+  <si>
     <t>F000000255</t>
   </si>
   <si>
     <t>LU0266117927</t>
   </si>
   <si>
+    <t>Morgan Stanley US Advantage Fund AH EUR (T) </t>
+  </si>
+  <si>
     <t>F0000023SJ</t>
   </si>
   <si>
     <t>GB00B2PDRY03</t>
   </si>
   <si>
+    <t>First St.I.-St.I.A.Pac.Sust.Fd</t>
+  </si>
+  <si>
     <t>F00000QLUP</t>
   </si>
   <si>
     <t>LU0976565415</t>
+  </si>
+  <si>
+    <t>Templeton Asian Smaller Companies Fund</t>
+  </si>
+  <si>
+    <t>Gesamt Handelbar @ Hellobank ü. Direkthandel</t>
+  </si>
+  <si>
+    <t>Mindest</t>
+  </si>
+  <si>
+    <t>12% Jahresrendite</t>
+  </si>
+  <si>
+    <t>10% Jahresrendite</t>
+  </si>
+  <si>
+    <t>Morgan Stanley – Gibt es erst seit 2016</t>
+  </si>
+  <si>
+    <t>Reduzierte Fonds wegen Mindesteinsatz</t>
+  </si>
+  <si>
+    <t>11% Rendite</t>
+  </si>
+  <si>
+    <t>Ab 2015: Frankfurter Aktienfonds für Stiftungen TI</t>
+  </si>
+  <si>
+    <t>Noch reduziertere Fonds wegen Mindesteinsatz</t>
   </si>
   <si>
     <t>r</t>
@@ -522,7 +637,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -582,8 +697,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +721,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -658,16 +785,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -699,6 +826,18 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -707,7 +846,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Accent2" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Accent2" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -778,15 +917,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>211320</xdr:colOff>
+      <xdr:colOff>237960</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -801,8 +940,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5522760" cy="6481440"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5522400" cy="6481080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -822,15 +961,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>465120</xdr:colOff>
+      <xdr:colOff>491760</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -845,8 +984,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5776560" cy="5058360"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5776200" cy="5058000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -866,15 +1005,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>618840</xdr:colOff>
+      <xdr:colOff>645480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -889,8 +1028,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5930280" cy="5090760"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5929920" cy="5090400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -910,15 +1049,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>168480</xdr:colOff>
+      <xdr:colOff>195120</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -933,8 +1072,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="6242400" cy="5321160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="6242040" cy="5320800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -954,15 +1093,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>398520</xdr:colOff>
+      <xdr:colOff>425160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -977,8 +1116,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5709960" cy="4891680"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5709600" cy="4891320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,15 +1137,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>34560</xdr:colOff>
+      <xdr:colOff>61560</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>448200</xdr:colOff>
+      <xdr:colOff>474840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1021,8 +1160,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="34560" y="0"/>
-          <a:ext cx="6514560" cy="5549760"/>
+          <a:off x="61560" y="0"/>
+          <a:ext cx="6514200" cy="5549400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1042,15 +1181,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>159480</xdr:colOff>
+      <xdr:colOff>186120</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1065,8 +1204,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="6233400" cy="5163120"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="6233040" cy="5162760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1086,15 +1225,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>148680</xdr:colOff>
+      <xdr:colOff>175320</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1109,8 +1248,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="6222600" cy="5186160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="6222240" cy="5185800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1130,15 +1269,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>525960</xdr:colOff>
+      <xdr:colOff>552600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1153,8 +1292,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5074560" cy="6098400"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5074200" cy="6098040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1174,15 +1313,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>261720</xdr:colOff>
+      <xdr:colOff>288360</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1197,8 +1336,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="6335640" cy="5332680"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="6335280" cy="5332320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1218,15 +1357,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>569880</xdr:colOff>
+      <xdr:colOff>596520</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1241,8 +1380,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5881320" cy="5060160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5880960" cy="5059800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1262,15 +1401,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>618480</xdr:colOff>
+      <xdr:colOff>645120</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1285,8 +1424,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5929920" cy="5176440"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5929560" cy="5176080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,15 +1445,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>468000</xdr:colOff>
+      <xdr:colOff>494640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1329,8 +1468,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5779440" cy="5009040"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5779080" cy="5008680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1350,15 +1489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>481320</xdr:colOff>
+      <xdr:colOff>507960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1373,8 +1512,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="5792760" cy="5054760"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="5792400" cy="5054400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1394,15 +1533,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1417,8 +1556,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="6204240" cy="5157360"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="6203880" cy="5157000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1438,15 +1577,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>42120</xdr:colOff>
+      <xdr:colOff>69120</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>308520</xdr:colOff>
+      <xdr:colOff>335160</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1461,8 +1600,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="42120" y="0"/>
-          <a:ext cx="5604840" cy="4940280"/>
+          <a:off x="69120" y="0"/>
+          <a:ext cx="5604480" cy="4939920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1482,561 +1621,1769 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.663967611336"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.4493927125506"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4372469635628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.09311740890688"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.9676113360324"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.9676113360324"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.9757085020243"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="M1" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>858</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>100000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="M15" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>100</v>
+        <v>111</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>105</v>
+        <v>117</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>110</v>
+        <v>122</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>114</v>
+        <v>127</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>129</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>119</v>
+        <v>131</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>124</v>
+        <v>137</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M29" s="0" t="s">
-        <v>128</v>
+        <v>140</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="M30" s="0" t="s">
-        <v>132</v>
+        <v>145</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C35" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>136</v>
+        <v>151</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>138</v>
+        <v>155</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>163</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>167</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>171</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>148</v>
+        <v>174</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
+        <v>180</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <f aca="false">$L$49*J51</f>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0.0837</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>0.0971</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <f aca="false">$L$49*J52</f>
+        <v>873.9</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <f aca="false">$L$49*J53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>0.0937</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>0.1297</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <f aca="false">$L$49*J54</f>
+        <v>1167.3</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>0.0093</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <f aca="false">$L$49*J55</f>
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>0.0849</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>0.0746</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <f aca="false">$L$49*J56</f>
+        <v>671.4</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>0.0824</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>0.0809</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <f aca="false">$L$49*J57</f>
+        <v>728.1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>0.0746</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>0.0682</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <f aca="false">$L$49*J58</f>
+        <v>613.8</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <f aca="false">$L$49*J59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>0.0783</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>0.0513</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <f aca="false">$L$49*J60</f>
+        <v>461.7</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="11" t="n">
+        <v>858</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>0.0632</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>0.0362</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">$L$49*J61</f>
+        <v>325.8</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <f aca="false">$L$49*J62</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>0.0525</v>
+      </c>
+      <c r="J63" s="0" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <f aca="false">$L$49*J63</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>0.0604</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>0.0665</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <f aca="false">$L$49*J64</f>
+        <v>598.5</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <f aca="false">$L$49*J65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <f aca="false">$L$49*J66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>0.0857</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>0.0605</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <f aca="false">$L$49*J67</f>
+        <v>544.5</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <f aca="false">$L$49*J68</f>
+        <v>137.7</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>0.0529</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>0.0867</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <f aca="false">$L$49*J69</f>
+        <v>780.3</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>0.0644</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>0.0945</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <f aca="false">$L$49*J70</f>
+        <v>850.5</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>0.0719</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>0.0522</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <f aca="false">$L$49*J71</f>
+        <v>469.8</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <f aca="false">$I$75*G76</f>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>0.0973</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <f aca="false">$I$75*G77</f>
+        <v>875.7</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B78" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <f aca="false">$I$75*G78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>0.0822</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <f aca="false">$I$75*G79</f>
+        <v>739.8</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>0.0609</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <f aca="false">$I$75*G80</f>
+        <v>548.1</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>0.0989</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <f aca="false">$I$75*G81</f>
+        <v>890.1</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>0.0957</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <f aca="false">$I$75*G82</f>
+        <v>861.3</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>0.0782</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <f aca="false">$I$75*G83</f>
+        <v>703.8</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>0.0645</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <f aca="false">$I$75*G84</f>
+        <v>580.5</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" s="11" t="n">
+        <v>858</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>0.0383</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <f aca="false">$I$75*G85</f>
+        <v>344.7</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <v>0.0103</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <f aca="false">$I$75*G86</f>
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G87" s="0" t="n">
+        <v>0.0794</v>
+      </c>
+      <c r="I87" s="0" t="n">
+        <f aca="false">$I$75*G87</f>
+        <v>714.6</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B88" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G88" s="0" t="n">
+        <v>0.0659</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <f aca="false">$I$75*G88</f>
+        <v>593.1</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" s="0" t="n">
+        <f aca="false">$I$75*G89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <f aca="false">$I$75*G90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G91" s="0" t="n">
+        <v>0.0368</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <f aca="false">$I$75*G91</f>
+        <v>331.2</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <v>0.0404</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <f aca="false">$I$75*G92</f>
+        <v>363.6</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B93" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <v>0.0859</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <f aca="false">$I$75*G93</f>
+        <v>773.1</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G94" s="0" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <f aca="false">$I$75*G94</f>
+        <v>128.7</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>0.057</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>0.0766</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B100" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>0.1529</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B102" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F102" s="0" t="n">
+        <v>0.0242</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <v>0.1541</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" s="0" t="n">
+        <v>0.0338</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B105" s="11" t="n">
+        <v>858</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>0.0696</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B106" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>0.0558</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B107" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>0.0613</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B108" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>0.0693</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <v>0.0787</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B113" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>0.1668</v>
+      </c>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I4" location="'MSIF Asia Opportunity AH EUR'!A1" display="MSIF Asia Opportunity AH EUR'!A1"/>
@@ -2063,7 +3410,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2090,7 +3437,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2117,7 +3464,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2144,7 +3491,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2169,42 +3516,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="I16"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
-  </cols>
-  <sheetData>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2224,6 +3538,39 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="I16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2231,7 +3578,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2256,9 +3603,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A3:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2269,24 +3643,24 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2300,14 +3674,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2334,23 +3708,22 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2361,8 +3734,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2388,8 +3761,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2415,7 +3788,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2442,7 +3815,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2469,7 +3842,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2496,7 +3869,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2523,7 +3896,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed the Difference between Mathematica and SciPy - This is a WIP Commit!
</commit_message>
<xml_diff>
--- a/Investment_Produkte_Details.xlsx
+++ b/Investment_Produkte_Details.xlsx
@@ -9,31 +9,32 @@
   </bookViews>
   <sheets>
     <sheet name="Allgemeines" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet19" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Kapital Plus A EUR" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Jupiter Europa L EUR B" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Mozart one R T" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Fidelity Fd.Glob.Technology" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="iShares ETF" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Fidelity Funds Germany" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="M&amp;G European Strategic Value C " sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Deutsche Invest I German Eq.FC " sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="BGF European Special Situati." sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="BGF Cont.European" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Fidelity Funds" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="BSF European Opport.Extension " sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="MainFirst Germany C" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="MSIF US Growth Z EUR" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="BGF World Technology" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Sheet2" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="MSIF Asia Opportunity AH EUR" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Sheet20" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet19" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Kapital Plus A EUR" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Jupiter Europa L EUR B" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Mozart one R T" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Fidelity Fd.Glob.Technology" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="iShares ETF" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Fidelity Funds Germany" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="M&amp;G European Strategic Value C " sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Deutsche Invest I German Eq.FC " sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="BGF European Special Situati." sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="BGF Cont.European" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Fidelity Funds" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="BSF European Opport.Extension " sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="MainFirst Germany C" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="MSIF US Growth Z EUR" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="BGF World Technology" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Sheet2" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="MSIF Asia Opportunity AH EUR" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="213">
   <si>
     <t>Fond Name</t>
   </si>
@@ -606,6 +607,51 @@
   </si>
   <si>
     <t>Noch reduziertere Fonds wegen Mindesteinsatz</t>
+  </si>
+  <si>
+    <t>10% Rendite</t>
+  </si>
+  <si>
+    <t>Aktienfond für Stiftungen</t>
+  </si>
+  <si>
+    <t>Fond_ID</t>
+  </si>
+  <si>
+    <t>Aktienfond für Stiftungen (Nicht Institutionell)</t>
+  </si>
+  <si>
+    <t>Noch noch reduziertere Fonds wegen Mindesteinsatz</t>
+  </si>
+  <si>
+    <t>Mischfonds Flexibel</t>
+  </si>
+  <si>
+    <t>Mischfond flexibel Global</t>
+  </si>
+  <si>
+    <t>Mischfond Flexibel – stetiger Wertzuwachs</t>
+  </si>
+  <si>
+    <t>Mischfond Defensiv Global</t>
+  </si>
+  <si>
+    <t>Aktienfond Global</t>
+  </si>
+  <si>
+    <t>Aktienfond USA Standardwerte Growth</t>
+  </si>
+  <si>
+    <t>Aktien Deutschland Nebenwerte</t>
+  </si>
+  <si>
+    <t>Mischfond Defensiv EUR Anliehen und 40% Aktien</t>
+  </si>
+  <si>
+    <t>Aktien Long / Short Europa</t>
+  </si>
+  <si>
+    <t>Aktien Asien ohne Japan | Nebenwerte</t>
   </si>
   <si>
     <t>r</t>
@@ -1621,15 +1667,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M65536"/>
+  <dimension ref="A1:O65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E159" activeCellId="0" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.9311740890688"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4372469635628"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.09311740890688"/>
@@ -2405,7 +2451,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="0" t="s">
         <v>154</v>
       </c>
       <c r="B51" s="11" t="s">
@@ -2426,7 +2472,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B52" s="11" t="s">
@@ -2447,7 +2493,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="0" t="s">
         <v>162</v>
       </c>
       <c r="B53" s="11" t="n">
@@ -2462,7 +2508,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -2483,7 +2529,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="0" t="s">
         <v>170</v>
       </c>
       <c r="B55" s="11" t="n">
@@ -2504,7 +2550,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="0" t="s">
         <v>173</v>
       </c>
       <c r="B56" s="11" t="n">
@@ -2525,7 +2571,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="0" t="s">
         <v>176</v>
       </c>
       <c r="B57" s="11" t="n">
@@ -2546,7 +2592,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="0" t="s">
         <v>179</v>
       </c>
       <c r="B58" s="11" t="s">
@@ -2567,7 +2613,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="0" t="s">
         <v>17</v>
       </c>
       <c r="B59" s="11" t="n">
@@ -2582,7 +2628,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="11" t="n">
@@ -2603,7 +2649,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="0" t="s">
         <v>31</v>
       </c>
       <c r="B61" s="11" t="n">
@@ -2624,7 +2670,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B62" s="11" t="n">
@@ -2645,7 +2691,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B63" s="11" t="n">
@@ -2666,7 +2712,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="0" t="s">
         <v>54</v>
       </c>
       <c r="B64" s="11" t="n">
@@ -2687,7 +2733,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="0" t="s">
         <v>93</v>
       </c>
       <c r="B65" s="11" t="n">
@@ -2708,7 +2754,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="0" t="s">
         <v>98</v>
       </c>
       <c r="B66" s="11" t="s">
@@ -2729,7 +2775,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="0" t="s">
         <v>106</v>
       </c>
       <c r="B67" s="11" t="n">
@@ -2750,7 +2796,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="0" t="s">
         <v>118</v>
       </c>
       <c r="B68" s="11" t="n">
@@ -2771,7 +2817,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="0" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="11" t="n">
@@ -2792,7 +2838,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="0" t="s">
         <v>128</v>
       </c>
       <c r="B70" s="11" t="s">
@@ -2813,7 +2859,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="0" t="s">
         <v>146</v>
       </c>
       <c r="B71" s="11" t="n">
@@ -3195,6 +3241,9 @@
       <c r="B97" s="10" t="s">
         <v>183</v>
       </c>
+      <c r="H97" s="0" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="11" t="s">
@@ -3209,6 +3258,9 @@
       <c r="F98" s="0" t="n">
         <v>0.057</v>
       </c>
+      <c r="H98" s="0" t="n">
+        <v>0.0908</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="11" t="s">
@@ -3223,6 +3275,9 @@
       <c r="F99" s="0" t="n">
         <v>0.0766</v>
       </c>
+      <c r="H99" s="0" t="n">
+        <v>0.1762</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="11" t="s">
@@ -3248,6 +3303,9 @@
       <c r="F101" s="0" t="n">
         <v>0.1529</v>
       </c>
+      <c r="H101" s="0" t="n">
+        <v>0.1921</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11" t="s">
@@ -3262,6 +3320,9 @@
       <c r="F102" s="0" t="n">
         <v>0.0242</v>
       </c>
+      <c r="H102" s="0" t="n">
+        <v>0.0048</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
@@ -3276,19 +3337,8 @@
       <c r="F103" s="0" t="n">
         <v>0.1541</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B104" s="11" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" s="0" t="n">
-        <v>0.0338</v>
+      <c r="H103" s="0" t="n">
+        <v>0.0377</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3304,6 +3354,9 @@
       <c r="F105" s="0" t="n">
         <v>0.0696</v>
       </c>
+      <c r="H105" s="0" t="n">
+        <v>0.1454</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="11" t="s">
@@ -3318,6 +3371,9 @@
       <c r="F106" s="0" t="n">
         <v>0.0558</v>
       </c>
+      <c r="H106" s="0" t="n">
+        <v>0.0046</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
@@ -3332,6 +3388,9 @@
       <c r="F107" s="0" t="n">
         <v>0.0613</v>
       </c>
+      <c r="H107" s="0" t="n">
+        <v>0.1387</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="11" t="s">
@@ -3346,6 +3405,9 @@
       <c r="F108" s="0" t="n">
         <v>0.0693</v>
       </c>
+      <c r="H108" s="0" t="n">
+        <v>0.0442</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="11" t="s">
@@ -3360,6 +3422,37 @@
       <c r="F109" s="0" t="n">
         <v>0.0787</v>
       </c>
+      <c r="H109" s="0" t="n">
+        <v>0.1086</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B112" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="H112" s="0" t="n">
+        <v>0.0568</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="11" t="s">
@@ -3375,6 +3468,692 @@
         <v>0.1668</v>
       </c>
     </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="I119" s="0" t="n">
+        <v>0.1175</v>
+      </c>
+      <c r="J119" s="0" t="n">
+        <v>0.1041</v>
+      </c>
+      <c r="K119" s="0" t="n">
+        <v>0.0908</v>
+      </c>
+      <c r="L119" s="0" t="n">
+        <v>0.0776</v>
+      </c>
+      <c r="M119" s="0" t="n">
+        <v>0.0645</v>
+      </c>
+      <c r="N119" s="0" t="n">
+        <v>0.0515</v>
+      </c>
+      <c r="O119" s="0" t="n">
+        <v>0.0386</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="I120" s="0" t="n">
+        <v>0.1138</v>
+      </c>
+      <c r="J120" s="0" t="n">
+        <v>0.1035</v>
+      </c>
+      <c r="K120" s="0" t="n">
+        <v>0.0933</v>
+      </c>
+      <c r="L120" s="0" t="n">
+        <v>0.0832</v>
+      </c>
+      <c r="M120" s="0" t="n">
+        <v>0.0732</v>
+      </c>
+      <c r="N120" s="0" t="n">
+        <v>0.0632</v>
+      </c>
+      <c r="O120" s="0" t="n">
+        <v>0.0534</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B121" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="I121" s="0" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="J121" s="0" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="K121" s="0" t="n">
+        <v>0.1491</v>
+      </c>
+      <c r="L121" s="0" t="n">
+        <v>0.1432</v>
+      </c>
+      <c r="M121" s="0" t="n">
+        <v>0.1373</v>
+      </c>
+      <c r="N121" s="0" t="n">
+        <v>0.1315</v>
+      </c>
+      <c r="O121" s="0" t="n">
+        <v>0.1258</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="I122" s="0" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="J122" s="0" t="n">
+        <v>0.1588</v>
+      </c>
+      <c r="K122" s="0" t="n">
+        <v>0.1417</v>
+      </c>
+      <c r="L122" s="0" t="n">
+        <v>0.1247</v>
+      </c>
+      <c r="M122" s="0" t="n">
+        <v>0.1079</v>
+      </c>
+      <c r="N122" s="0" t="n">
+        <v>0.0912</v>
+      </c>
+      <c r="O122" s="0" t="n">
+        <v>0.0746</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="I123" s="0" t="n">
+        <v>0.0983</v>
+      </c>
+      <c r="J123" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="K123" s="0" t="n">
+        <v>0.1216</v>
+      </c>
+      <c r="L123" s="0" t="n">
+        <v>0.1332</v>
+      </c>
+      <c r="M123" s="0" t="n">
+        <v>0.1447</v>
+      </c>
+      <c r="N123" s="0" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="O123" s="0" t="n">
+        <v>0.1673</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B124" s="11" t="n">
+        <v>858</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="I124" s="0" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="J124" s="0" t="n">
+        <v>0.0539</v>
+      </c>
+      <c r="K124" s="0" t="n">
+        <v>0.0736</v>
+      </c>
+      <c r="L124" s="0" t="n">
+        <v>0.0932</v>
+      </c>
+      <c r="M124" s="0" t="n">
+        <v>0.1127</v>
+      </c>
+      <c r="N124" s="0" t="n">
+        <v>0.132</v>
+      </c>
+      <c r="O124" s="0" t="n">
+        <v>0.1512</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B125" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="I125" s="0" t="n">
+        <v>0.0193</v>
+      </c>
+      <c r="J125" s="0" t="n">
+        <v>0.0365</v>
+      </c>
+      <c r="K125" s="0" t="n">
+        <v>0.0536</v>
+      </c>
+      <c r="L125" s="0" t="n">
+        <v>0.0706</v>
+      </c>
+      <c r="M125" s="0" t="n">
+        <v>0.0875</v>
+      </c>
+      <c r="N125" s="0" t="n">
+        <v>0.1042</v>
+      </c>
+      <c r="O125" s="0" t="n">
+        <v>0.1208</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B126" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I126" s="0" t="n">
+        <v>0.0971</v>
+      </c>
+      <c r="J126" s="0" t="n">
+        <v>0.1126</v>
+      </c>
+      <c r="K126" s="0" t="n">
+        <v>0.1279</v>
+      </c>
+      <c r="L126" s="0" t="n">
+        <v>0.1431</v>
+      </c>
+      <c r="M126" s="0" t="n">
+        <v>0.1582</v>
+      </c>
+      <c r="N126" s="0" t="n">
+        <v>0.1732</v>
+      </c>
+      <c r="O126" s="0" t="n">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="I127" s="0" t="n">
+        <v>0.1831</v>
+      </c>
+      <c r="J127" s="0" t="n">
+        <v>0.1656</v>
+      </c>
+      <c r="K127" s="0" t="n">
+        <v>0.1483</v>
+      </c>
+      <c r="L127" s="0" t="n">
+        <v>0.1311</v>
+      </c>
+      <c r="M127" s="0" t="n">
+        <v>0.1141</v>
+      </c>
+      <c r="N127" s="0" t="n">
+        <v>0.0972</v>
+      </c>
+      <c r="O127" s="0" t="n">
+        <v>0.0804</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B129" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B130" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B138" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G138" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B139" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G139" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B140" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B141" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G141" s="0" t="n">
+        <v>0.2917</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B142" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C142" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G142" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B143" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G143" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B144" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G144" s="0" t="n">
+        <v>0.1193</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="G145" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G147" s="0" t="n">
+        <v>0.1202</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B148" s="11" t="n">
+        <v>858</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G148" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B149" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B150" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B151" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G151" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B152" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G152" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B153" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G153" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B154" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G154" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B155" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B156" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G156" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B157" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B158" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G158" s="0" t="n">
+        <v>0.4688</v>
+      </c>
+    </row>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3543,23 +4322,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="I16"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
   </cols>
-  <sheetData>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3576,17 +4349,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="I16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3630,6 +4409,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A3:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -3643,24 +4449,24 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3674,7 +4480,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3701,7 +4554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3727,7 +4580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3754,7 +4607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3763,33 +4616,6 @@
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added the Optimization for All Products again and ran the Optimization.
</commit_message>
<xml_diff>
--- a/Investment_Produkte_Details.xlsx
+++ b/Investment_Produkte_Details.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="226">
   <si>
     <t>Fond Name</t>
   </si>
@@ -652,6 +652,45 @@
   </si>
   <si>
     <t>Aktien Asien ohne Japan | Nebenwerte</t>
+  </si>
+  <si>
+    <t>Reduzierte Fonds Handelbar @ Hellobank ü. Direkthandel</t>
+  </si>
+  <si>
+    <t>10%Rendite</t>
+  </si>
+  <si>
+    <t>Institutionell?</t>
+  </si>
+  <si>
+    <t>(Amerikanische Aktien)</t>
+  </si>
+  <si>
+    <t>Aktien USA Standardwerte</t>
+  </si>
+  <si>
+    <t>Mischfond Euro Flexibel</t>
+  </si>
+  <si>
+    <t>Keine Grenze (A-H Klasse)</t>
+  </si>
+  <si>
+    <t>1500 minimal (E-Klasse, Spesen)</t>
+  </si>
+  <si>
+    <t>1.513,36</t>
+  </si>
+  <si>
+    <t>1000 Minimal</t>
+  </si>
+  <si>
+    <t>LU0266117414</t>
+  </si>
+  <si>
+    <t>1500 minimal</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
   <si>
     <t>r</t>
@@ -679,9 +718,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -831,7 +871,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -882,6 +922,14 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1669,8 +1717,8 @@
   </sheetPr>
   <dimension ref="A1:O65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E159" activeCellId="0" sqref="E159"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C202" activeCellId="0" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3890,38 +3938,41 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B140" s="11" t="n">
-        <v>1000</v>
+        <v>166</v>
+      </c>
+      <c r="B140" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="G140" s="0" t="n">
+        <v>0.2917</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B141" s="11" t="s">
-        <v>100</v>
+        <v>170</v>
+      </c>
+      <c r="B141" s="11" t="n">
+        <v>1500</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G141" s="0" t="n">
-        <v>0.2917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B142" s="11" t="n">
         <v>1500</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G142" s="0" t="n">
         <v>0</v>
@@ -3929,41 +3980,41 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B143" s="11" t="n">
         <v>1500</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G143" s="0" t="n">
-        <v>0</v>
+        <v>0.1193</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B144" s="11" t="n">
-        <v>1500</v>
+        <v>179</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G144" s="0" t="n">
-        <v>0.1193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B145" s="11" t="s">
-        <v>100</v>
+        <v>24</v>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>1500</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>181</v>
+        <v>19</v>
       </c>
       <c r="G145" s="0" t="n">
         <v>0</v>
@@ -3971,41 +4022,41 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B146" s="11" t="n">
-        <v>1500</v>
+        <v>858</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="G146" s="0" t="n">
-        <v>0</v>
+        <v>0.1202</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B147" s="11" t="n">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G147" s="0" t="n">
-        <v>0.1202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B148" s="11" t="n">
-        <v>858</v>
+        <v>1500</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="G148" s="0" t="n">
         <v>0</v>
@@ -4013,13 +4064,13 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B149" s="11" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G149" s="0" t="n">
         <v>0</v>
@@ -4027,13 +4078,13 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="B150" s="11" t="n">
         <v>1500</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="G150" s="0" t="n">
         <v>0</v>
@@ -4041,13 +4092,13 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B151" s="11" t="n">
-        <v>1500</v>
+        <v>98</v>
+      </c>
+      <c r="B151" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="G151" s="0" t="n">
         <v>0</v>
@@ -4055,13 +4106,13 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B152" s="11" t="n">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="G152" s="0" t="n">
         <v>0</v>
@@ -4069,13 +4120,13 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B153" s="11" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="B153" s="11" t="n">
+        <v>1500</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="G153" s="0" t="n">
         <v>0</v>
@@ -4083,13 +4134,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B154" s="11" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="G154" s="0" t="n">
         <v>0</v>
@@ -4097,13 +4148,13 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B155" s="11" t="n">
-        <v>1500</v>
+        <v>128</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="G155" s="0" t="n">
         <v>0</v>
@@ -4111,13 +4162,13 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B156" s="11" t="n">
         <v>1500</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="G156" s="0" t="n">
         <v>0</v>
@@ -4125,32 +4176,655 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B157" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>0.4688</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B161" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C161" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G161" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B164" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G164" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="H164" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="I164" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="J164" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G165" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="H165" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="I165" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="J165" s="0" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B166" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <v>0.358</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <v>0.3896</v>
+      </c>
+      <c r="I168" s="0" t="n">
+        <v>0.355</v>
+      </c>
+      <c r="J168" s="0" t="n">
+        <v>0.3862</v>
+      </c>
+      <c r="K168" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B169" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H169" s="0" t="n">
+        <v>0.0271</v>
+      </c>
+      <c r="I169" s="0" t="n">
+        <v>0.0968</v>
+      </c>
+      <c r="J169" s="0" t="n">
+        <v>0.0594</v>
+      </c>
+      <c r="K169" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B170" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K170" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B171" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="G171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H171" s="0" t="n">
+        <v>0.0218</v>
+      </c>
+      <c r="I171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J171" s="0" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="K171" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B172" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I172" s="0" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="J172" s="0" t="n">
+        <v>0.1184</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B173" s="11" t="n">
+        <v>858</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G173" s="0" t="n">
+        <v>0.1824</v>
+      </c>
+      <c r="H173" s="0" t="n">
+        <v>0.1057</v>
+      </c>
+      <c r="I173" s="0" t="n">
+        <v>0.0644</v>
+      </c>
+      <c r="J173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K173" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B174" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" s="0" t="n">
+        <v>0.0452</v>
+      </c>
+      <c r="I174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J174" s="0" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="K174" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B175" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J175" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B176" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J176" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B177" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J177" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B178" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J178" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B179" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H179" s="0" t="n">
+        <v>0.1273</v>
+      </c>
+      <c r="I179" s="0" t="n">
+        <v>0.1512</v>
+      </c>
+      <c r="J179" s="0" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="K179" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B180" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J180" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B181" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" s="0" t="n">
+        <v>0.1567</v>
+      </c>
+      <c r="I181" s="0" t="n">
+        <v>0.2934</v>
+      </c>
+      <c r="J181" s="0" t="n">
+        <v>0.2365</v>
+      </c>
+      <c r="K181" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B157" s="11" t="s">
+      <c r="B182" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C157" s="0" t="s">
+      <c r="C182" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="G157" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
+      <c r="G182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J182" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B158" s="11" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C158" s="0" t="s">
+      <c r="B183" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C183" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="G158" s="0" t="n">
-        <v>0.4688</v>
-      </c>
-    </row>
+      <c r="G183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J183" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B184" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="G184" s="0" t="n">
+        <v>0.4596</v>
+      </c>
+      <c r="H184" s="0" t="n">
+        <v>0.1266</v>
+      </c>
+      <c r="I184" s="0" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="J184" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K184" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="M184" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F188" s="0" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E189" s="14"/>
+      <c r="F189" s="14"/>
+    </row>
+    <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="E190" s="14" t="n">
+        <f aca="false">F190/$F$188</f>
+        <v>0.3</v>
+      </c>
+      <c r="F190" s="14" t="n">
+        <f aca="false">8000*0.3</f>
+        <v>2400</v>
+      </c>
+      <c r="G190" s="0" t="str">
+        <f aca="false">C168</f>
+        <v>M&amp;G OPTIMAL INCOME FUND (T)</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E191" s="14" t="n">
+        <f aca="false">F191/$F$188</f>
+        <v>0.1875</v>
+      </c>
+      <c r="F191" s="14" t="n">
+        <f aca="false">500*3</f>
+        <v>1500</v>
+      </c>
+      <c r="G191" s="0" t="str">
+        <f aca="false">C179</f>
+        <v>Fidelity Fd.Glob.Technology A Dis EUR </v>
+      </c>
+      <c r="L191" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E192" s="14" t="n">
+        <f aca="false">F192/$F$188</f>
+        <v>0.32</v>
+      </c>
+      <c r="F192" s="14" t="n">
+        <f aca="false">F188*0.32</f>
+        <v>2560</v>
+      </c>
+      <c r="G192" s="0" t="str">
+        <f aca="false">C184</f>
+        <v>Aktienfond für Stiftungen (Nicht Institutionell)</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C193" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="E193" s="14" t="n">
+        <f aca="false">F193/$F$188</f>
+        <v>0.2145</v>
+      </c>
+      <c r="F193" s="11" t="n">
+        <f aca="false">858*2</f>
+        <v>1716</v>
+      </c>
+      <c r="G193" s="0" t="str">
+        <f aca="false">C173</f>
+        <v>MSIF US Growth Z EUR</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E194" s="14"/>
+      <c r="F194" s="14"/>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E195" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="F195" s="14" t="n">
+        <f aca="false">SUM(F190:F193)</f>
+        <v>8176</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C199" s="0" t="n">
+        <f aca="false">2060-1513.36</f>
+        <v>546.64</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C201" s="0" t="n">
+        <f aca="false">F195-2060</f>
+        <v>6116</v>
+      </c>
+    </row>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4362,7 +5036,7 @@
   <sheetData>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I16" s="0" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -4449,24 +5123,24 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>